<commit_message>
Added SMPBART output for glass,vertebral. Added script for Friedman Smooth DGP simulation.
</commit_message>
<xml_diff>
--- a/output/rf_glass_output.xlsx
+++ b/output/rf_glass_output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5cac48941448979/Bureaublad/msc_thesis/thesis_code/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_42CED8002847A1812ABC23EF38953BEDE9E2A164" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26059D7-68F6-40D6-84BB-A87D6B24ECFA}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_42CED8002877ABEECA3F22EF38953BEDE9E2A164" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A6AB49-0AA4-410F-A137-1A3B5547929F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misclassification_rates" sheetId="1" r:id="rId1"/>
@@ -375,6 +375,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0.232558139534884</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0.232558139534884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.13953488372093001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.19047619047618999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.232558139534884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f>AVERAGE(A1:A5)</f>
+        <v>0.2055370985603544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>_xlfn.STDEV.S(A1:A5)</f>
+        <v>4.1150739003299838E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
@@ -383,65 +442,6 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>0.232558139534884</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>0.232558139534884</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0.13953488372093001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0.19047619047618999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0.232558139534884</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <f>AVERAGE(A1:A5)</f>
-        <v>0.2055370985603544</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <f>_xlfn.STDEV.S(A1:A5)</f>
-        <v>4.1150739003299838E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
         <v>0.27867274418604698</v>
       </c>
     </row>

</xml_diff>